<commit_message>
updated changes in dumpscript file
</commit_message>
<xml_diff>
--- a/Task_3/src/script/data.xlsx
+++ b/Task_3/src/script/data.xlsx
@@ -88,7 +88,7 @@
     <t>nand</t>
   </si>
   <si>
-    <t>sree clinic</t>
+    <t>sreeclinic</t>
   </si>
   <si>
     <t>soumysree@gmail.com</t>
@@ -135,18 +135,18 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -199,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -207,35 +207,44 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,19 +573,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +613,7 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -624,19 +633,19 @@
       <c r="E2" s="2">
         <v>36064</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="5">
         <v>9550717673</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -656,19 +665,19 @@
       <c r="E3" s="2">
         <v>35953</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="5">
         <v>9865457667</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -688,19 +697,19 @@
       <c r="E4" s="2">
         <v>35938</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="5">
         <v>8786764322</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -720,81 +729,81 @@
       <c r="E5" s="2">
         <v>37460</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>45</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <v>9897864348</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="I7" s="8"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="I8" s="8"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="I9" s="8"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1"/>
@@ -802,11 +811,11 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="9"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1"/>
@@ -814,11 +823,11 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="7"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1"/>
@@ -826,11 +835,11 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1"/>
@@ -838,11 +847,11 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="9"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1"/>
@@ -850,11 +859,11 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="7"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1"/>
@@ -862,11 +871,11 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1"/>
@@ -874,11 +883,11 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="9"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>